<commit_message>
Teste07 - Com excel ok
</commit_message>
<xml_diff>
--- a/dados_extraidos.xlsx
+++ b/dados_extraidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M\Documents\GitHub\automacaoPythonAvanttiChips\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB3C2E7-C6B9-42E0-AC2C-BE197A1F59E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFBFF40-5859-4612-B2BB-8F913F18AAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
   <si>
     <t>Quantos cartão</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>EDUARDO JOSE SOARES BRANDAO</t>
+  </si>
+  <si>
+    <t>(73) 9 8824-8659</t>
   </si>
 </sst>
 </file>
@@ -193,12 +196,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -230,7 +239,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -535,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,6 +560,7 @@
     <col min="6" max="8" width="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="51.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -809,6 +819,41 @@
         <v>50</v>
       </c>
     </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>